<commit_message>
Update Excel template Kipo_Project_Form.xlsx
</commit_message>
<xml_diff>
--- a/Kipo_Project_Form.xlsx
+++ b/Kipo_Project_Form.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Kevin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Python\Project_Form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A6736D8-001D-498D-9338-1133F15D01D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C0D7E9-DC84-4E02-9F36-0A5D45D68D4E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>Kipo科普科技股份有限公司
 電話：+886-2-8522-7278
@@ -152,10 +152,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>北辦工程</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>產品應用</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -205,17 +201,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">業務主管：
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">研發主管：
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>申請人簽名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>業務主管</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>研發主管</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -223,7 +217,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,13 +247,6 @@
       <charset val="136"/>
     </font>
     <font>
-      <sz val="15"/>
-      <color theme="1"/>
-      <name val="標楷體"/>
-      <family val="4"/>
-      <charset val="136"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="新細明體"/>
@@ -281,25 +268,18 @@
       <charset val="136"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="新細明體"/>
-      <family val="1"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="20"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="標楷體"/>
       <family val="4"/>
       <charset val="136"/>
     </font>
     <font>
-      <sz val="18"/>
+      <sz val="24"/>
       <color theme="1"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="標楷體"/>
+      <family val="4"/>
+      <charset val="136"/>
     </font>
   </fonts>
   <fills count="3">
@@ -606,7 +586,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -626,21 +606,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -649,157 +670,90 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1482,302 +1436,302 @@
   </sheetPr>
   <dimension ref="A1:V23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:F13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="30.69921875" customWidth="1"/>
+    <col min="1" max="6" width="30.69921875" style="50" customWidth="1"/>
+    <col min="7" max="16384" width="8.796875" style="50"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30"/>
-      <c r="B1" s="31"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="39" t="s">
+      <c r="A1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="41"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="33"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="44"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" spans="1:22" ht="24.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="36"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="47"/>
-    </row>
-    <row r="4" spans="1:22" ht="28" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="48" t="s">
+      <c r="A3" s="21"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="32"/>
+    </row>
+    <row r="4" spans="1:22" ht="34" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="50"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
-    </row>
-    <row r="5" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="17" t="s">
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="45"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="51"/>
+      <c r="R4" s="51"/>
+      <c r="S4" s="51"/>
+      <c r="T4" s="51"/>
+      <c r="U4" s="51"/>
+      <c r="V4" s="51"/>
+    </row>
+    <row r="5" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="17" t="s">
+      <c r="B5" s="37"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="39"/>
+    </row>
+    <row r="6" spans="1:22" ht="25.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="42"/>
+    </row>
+    <row r="7" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="37"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="37"/>
+      <c r="F7" s="39"/>
+    </row>
+    <row r="8" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="38"/>
+      <c r="F8" s="39"/>
+    </row>
+    <row r="9" spans="1:22" ht="52.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="52"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="34"/>
+    </row>
+    <row r="10" spans="1:22" ht="25.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="36"/>
+    </row>
+    <row r="11" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="65"/>
-      <c r="F5" s="66"/>
-    </row>
-    <row r="6" spans="1:22" ht="22" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="67" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="68"/>
-    </row>
-    <row r="7" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="63"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="65"/>
-      <c r="F7" s="66"/>
-    </row>
-    <row r="8" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="28"/>
-      <c r="F8" s="29"/>
-    </row>
-    <row r="9" spans="1:22" ht="52.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="21"/>
-    </row>
-    <row r="10" spans="1:22" ht="22" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="60" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="61"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="62"/>
-    </row>
-    <row r="11" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="16" t="s">
+      <c r="B11" s="37"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="17" t="s">
+      <c r="E11" s="37"/>
+      <c r="F11" s="39"/>
+    </row>
+    <row r="12" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="65"/>
-      <c r="F11" s="66"/>
-    </row>
-    <row r="12" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="16" t="s">
+      <c r="B12" s="37"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="63"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="17" t="s">
+      <c r="E12" s="37"/>
+      <c r="F12" s="39"/>
+    </row>
+    <row r="13" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="65"/>
-      <c r="F12" s="66"/>
-    </row>
-    <row r="13" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="16" t="s">
+      <c r="B13" s="37"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="63"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="17" t="s">
+      <c r="E13" s="37"/>
+      <c r="F13" s="39"/>
+    </row>
+    <row r="14" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="65"/>
-      <c r="F13" s="66"/>
-    </row>
-    <row r="14" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="16" t="s">
+      <c r="B14" s="37"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="37"/>
+      <c r="F14" s="39"/>
+    </row>
+    <row r="15" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="70"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="17" t="s">
+      <c r="B15" s="37"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="71"/>
-      <c r="F14" s="72"/>
-    </row>
-    <row r="15" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="69" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="70"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="17" t="s">
+      <c r="E15" s="37"/>
+      <c r="F15" s="39"/>
+    </row>
+    <row r="16" spans="1:22" ht="25.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="36"/>
+    </row>
+    <row r="17" spans="1:6" ht="400" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="47"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="49"/>
+    </row>
+    <row r="18" spans="1:6" ht="25.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="71"/>
-      <c r="F15" s="72"/>
-    </row>
-    <row r="16" spans="1:22" ht="22" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="60" t="s">
+      <c r="B18" s="46"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="36"/>
+    </row>
+    <row r="19" spans="1:6" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="59"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="61"/>
+    </row>
+    <row r="20" spans="1:6" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="59"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="61"/>
+    </row>
+    <row r="21" spans="1:6" ht="52.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="56"/>
+      <c r="E21" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="39"/>
+    </row>
+    <row r="22" spans="1:6" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="63"/>
+      <c r="B22" s="64"/>
+      <c r="C22" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="61"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="62"/>
-    </row>
-    <row r="17" spans="1:6" ht="234" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="22"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="26"/>
-    </row>
-    <row r="18" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="60" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="61"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="61"/>
-      <c r="F18" s="62"/>
-    </row>
-    <row r="19" spans="1:6" ht="136" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="24"/>
-    </row>
-    <row r="20" spans="1:6" ht="136" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="24"/>
-    </row>
-    <row r="21" spans="1:6" ht="52.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="F21" s="52"/>
-    </row>
-    <row r="22" spans="1:6" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A22" s="54"/>
-      <c r="B22" s="55"/>
-      <c r="C22" s="56" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="56"/>
-      <c r="E22" s="56" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" s="56"/>
-    </row>
-    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="57" t="s">
+      <c r="F22" s="64"/>
+    </row>
+    <row r="23" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A23" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="58"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="58"/>
-      <c r="F23" s="59"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="31">
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="A17:B17"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E5:F5"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="B12:C12"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A1:C3"/>
+    <mergeCell ref="D1:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E7:F7"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A1:C3"/>
-    <mergeCell ref="D1:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Update Excel template for spec info formatting
</commit_message>
<xml_diff>
--- a/Kipo_Project_Form.xlsx
+++ b/Kipo_Project_Form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Python\Project_Form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C0D7E9-DC84-4E02-9F36-0A5D45D68D4E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BFB1C14-CA3C-4371-9C9B-A4B77AB26994}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -586,7 +586,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -610,6 +610,29 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -664,46 +687,52 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -712,32 +741,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -746,15 +767,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1437,267 +1449,267 @@
   <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="30.69921875" style="50" customWidth="1"/>
-    <col min="7" max="16384" width="8.796875" style="50"/>
+    <col min="1" max="6" width="30.69921875" style="15" customWidth="1"/>
+    <col min="7" max="16384" width="8.796875" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="24" t="s">
+      <c r="A1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="26"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="29"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:22" ht="24.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="21"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="32"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="41"/>
     </row>
     <row r="4" spans="1:22" ht="34" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="45"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="51"/>
-      <c r="P4" s="51"/>
-      <c r="Q4" s="51"/>
-      <c r="R4" s="51"/>
-      <c r="S4" s="51"/>
-      <c r="T4" s="51"/>
-      <c r="U4" s="51"/>
-      <c r="V4" s="51"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="44"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
     </row>
     <row r="5" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="39"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="22"/>
     </row>
     <row r="6" spans="1:22" ht="25.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="42"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="47"/>
     </row>
     <row r="7" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="56" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="37"/>
-      <c r="F7" s="39"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="22"/>
     </row>
     <row r="8" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="56" t="s">
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="38"/>
-      <c r="F8" s="39"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="22"/>
     </row>
     <row r="9" spans="1:22" ht="52.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="52"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="34"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="53"/>
     </row>
     <row r="10" spans="1:22" ht="25.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="36"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="64"/>
     </row>
     <row r="11" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="56" t="s">
+      <c r="B11" s="21"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="56" t="s">
+      <c r="B12" s="21"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="37"/>
-      <c r="F12" s="39"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="22"/>
     </row>
     <row r="13" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="56" t="s">
+      <c r="B13" s="21"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="37"/>
-      <c r="F13" s="39"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="22"/>
     </row>
     <row r="14" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="56" t="s">
+      <c r="B14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="37"/>
-      <c r="F14" s="39"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="22"/>
     </row>
     <row r="15" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="56" t="s">
+      <c r="B15" s="21"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="37"/>
-      <c r="F15" s="39"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22"/>
     </row>
     <row r="16" spans="1:22" ht="25.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="54" t="s">
         <v>40</v>
       </c>
       <c r="B16" s="46"/>
       <c r="C16" s="46"/>
       <c r="D16" s="46"/>
       <c r="E16" s="46"/>
-      <c r="F16" s="36"/>
+      <c r="F16" s="47"/>
     </row>
     <row r="17" spans="1:6" ht="400" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="47"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="49"/>
+      <c r="A17" s="58"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="65"/>
     </row>
     <row r="18" spans="1:6" ht="25.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="36"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="57"/>
     </row>
     <row r="19" spans="1:6" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="59"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="61"/>
+      <c r="B19" s="66"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="68"/>
     </row>
     <row r="20" spans="1:6" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="59"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="61"/>
+      <c r="B20" s="66"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="68"/>
     </row>
     <row r="21" spans="1:6" ht="52.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="62" t="s">
+      <c r="A21" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="56"/>
-      <c r="C21" s="56" t="s">
+      <c r="B21" s="17"/>
+      <c r="C21" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="56"/>
-      <c r="E21" s="37" t="s">
+      <c r="D21" s="17"/>
+      <c r="E21" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="39"/>
+      <c r="F21" s="22"/>
     </row>
     <row r="22" spans="1:6" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="63"/>
-      <c r="B22" s="64"/>
-      <c r="C22" s="64" t="s">
+      <c r="A22" s="61"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64" t="s">
+      <c r="D22" s="20"/>
+      <c r="E22" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="64"/>
+      <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="53" t="s">
+      <c r="A23" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="54"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="55"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="31">
@@ -1715,10 +1727,10 @@
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A10:F10"/>
     <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B12:C12"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="E11:F11"/>
     <mergeCell ref="A1:C3"/>
     <mergeCell ref="D1:F3"/>
     <mergeCell ref="A4:F4"/>
@@ -1729,8 +1741,8 @@
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="E13:F13"/>
-    <mergeCell ref="B14:C14"/>
     <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="E8:F8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
更新：B.開案資訊 SI/PV/MV/MP 改為 Schedule SI/PV/MV/MP，Google Sheet + Excel 模板同步一致
</commit_message>
<xml_diff>
--- a/Kipo_Project_Form.xlsx
+++ b/Kipo_Project_Form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Python\Project_Form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1EDFA0-0985-4D90-AA28-325B0299312A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24F1FC1-1EC5-4CEA-A3B6-C19082E4EE94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -177,22 +177,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Schedule_SI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Schedule_MV</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Schedule_PV</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Schedule_MP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>D.可行性評估</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -214,6 +198,22 @@
   </si>
   <si>
     <t>專案編號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Schedule SI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Schedule PV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Schedule MP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Schedule MV</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -628,6 +628,87 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -655,19 +736,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -702,75 +771,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1453,7 +1453,7 @@
   <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:F8"/>
+      <selection activeCell="A10" sqref="A10:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
@@ -1463,40 +1463,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="46"/>
-      <c r="B1" s="47"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="55" t="s">
+      <c r="A1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="56"/>
-      <c r="F1" s="57"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="60"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:22" ht="24.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="52"/>
-      <c r="B3" s="53"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="63"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="41"/>
     </row>
     <row r="4" spans="1:22" ht="34" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="66"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="44"/>
       <c r="N4" s="16"/>
       <c r="O4" s="16"/>
       <c r="P4" s="16"/>
@@ -1511,178 +1511,178 @@
       <c r="A5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="67"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="21"/>
       <c r="D5" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="67"/>
-      <c r="F5" s="31"/>
+        <v>40</v>
+      </c>
+      <c r="E5" s="21"/>
+      <c r="F5" s="22"/>
     </row>
     <row r="6" spans="1:22" ht="25.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="34"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="47"/>
     </row>
     <row r="7" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="31"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="22"/>
       <c r="D7" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="31"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="22"/>
     </row>
     <row r="8" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
       <c r="D8" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="67"/>
-      <c r="F8" s="31"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="22"/>
     </row>
     <row r="9" spans="1:22" ht="52.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="29"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="56"/>
     </row>
     <row r="10" spans="1:22" ht="25.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="44"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="67"/>
     </row>
     <row r="11" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="22"/>
       <c r="D11" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="30"/>
-      <c r="F11" s="31"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="31"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="31"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="22"/>
     </row>
     <row r="13" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="31"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="22"/>
       <c r="D13" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="31"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="22"/>
     </row>
     <row r="14" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="31"/>
+        <v>41</v>
+      </c>
+      <c r="B14" s="23"/>
+      <c r="C14" s="22"/>
       <c r="D14" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="31"/>
+        <v>42</v>
+      </c>
+      <c r="E14" s="23"/>
+      <c r="F14" s="22"/>
     </row>
     <row r="15" spans="1:22" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="23"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="23"/>
+      <c r="F15" s="22"/>
+    </row>
+    <row r="16" spans="1:22" ht="25.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="30"/>
-      <c r="F15" s="31"/>
-    </row>
-    <row r="16" spans="1:22" ht="25.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="34"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="47"/>
     </row>
     <row r="17" spans="1:6" ht="400" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="38"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="45"/>
+      <c r="A17" s="61"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="68"/>
     </row>
     <row r="18" spans="1:6" ht="25.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="37"/>
+      <c r="A18" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="60"/>
     </row>
     <row r="19" spans="1:6" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="23"/>
+        <v>38</v>
+      </c>
+      <c r="B19" s="48"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="50"/>
     </row>
     <row r="20" spans="1:6" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="23"/>
+        <v>39</v>
+      </c>
+      <c r="B20" s="48"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="50"/>
     </row>
     <row r="21" spans="1:6" ht="52.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="40" t="s">
+      <c r="A21" s="63" t="s">
         <v>1</v>
       </c>
       <c r="B21" s="17"/>
@@ -1690,35 +1690,51 @@
         <v>25</v>
       </c>
       <c r="D21" s="17"/>
-      <c r="E21" s="30" t="s">
+      <c r="E21" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="31"/>
+      <c r="F21" s="22"/>
     </row>
     <row r="22" spans="1:6" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="41"/>
+      <c r="A22" s="64"/>
       <c r="B22" s="20"/>
       <c r="C22" s="20" t="s">
         <v>26</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="20" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="26"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="E11:F11"/>
@@ -1735,22 +1751,6 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>